<commit_message>
Add new leader(s) to dataleaders_data.xlsx
</commit_message>
<xml_diff>
--- a/dataleaders_data.xlsx
+++ b/dataleaders_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S.C.H\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED3D52BD-EC4D-43EC-82BD-3A53D503A699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3898D2-EC88-4F9E-8B5B-8E149F75124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1CA20431-27E8-4654-B146-CF2DEABF58FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>YoRadwan</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC96376-891A-4C2C-AA2B-FBFF84BD1677}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +509,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{460AE2A6-6AF3-4E2A-80BD-475BF942E610}"/>

</xml_diff>

<commit_message>
Add password change feature for leaders and update data files
</commit_message>
<xml_diff>
--- a/dataleaders_data.xlsx
+++ b/dataleaders_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S.C.H\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3898D2-EC88-4F9E-8B5B-8E149F75124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE71D2E-AB86-4302-A069-291B663AA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1CA20431-27E8-4654-B146-CF2DEABF58FA}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update dataleaders_data.xlsx with latest leaders data
</commit_message>
<xml_diff>
--- a/dataleaders_data.xlsx
+++ b/dataleaders_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S.C.H\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0BB5B4-D4EE-4C34-A7DF-BBF1273E3F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B7AEB-30FE-4CFC-98F4-AD493C8460DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1CA20431-27E8-4654-B146-CF2DEABF58FA}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>yusfrdwn@outlook.com</t>
   </si>
   <si>
-    <t>Admin Sch</t>
+    <t>Admin</t>
   </si>
 </sst>
 </file>

</xml_diff>